<commit_message>
update phone number and total price
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PracticeFile\OrderProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2274F305-0228-45AE-8041-21790350C133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA1A252-9CFC-494A-8F42-7930C7FEEB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="975" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -158,25 +158,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> ( 1台斤 ± 10g )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ( 1台斤 ± 10g )</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (一隻 400g ± 10%)</t>
   </si>
   <si>
     <t>( 1.1Kg/盒 ）</t>
   </si>
   <si>
-    <t>煙燻花枝  ( 1台斤± 10g ) +
-熟小卷  ( 1台斤 ± 10g )</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>煙燻花枝  ( 1台斤 ± 10g )   +
- 熟小卷  ( 1台斤 ± 10g )  + 
+    <t xml:space="preserve"> ( 一台斤 ± 10% )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  ( 1台斤 ± 10% )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>煙燻花枝  ( 1台斤± 10% ) +
+熟小卷  ( 1台斤 ± 10% )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>煙燻花枝  ( 1台斤 ± 10% )   +
+ 熟小卷  ( 1台斤 ± 10% )  + 
 品元堂佛跳牆  ( 2200g )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -594,7 +596,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -622,7 +624,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>580</v>
@@ -636,7 +638,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>490</v>
@@ -664,7 +666,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2">
         <v>280</v>
@@ -678,7 +680,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2">
         <v>700</v>

</xml_diff>